<commit_message>
shading - compare FACS
</commit_message>
<xml_diff>
--- a/STORE_model/ML_model/data/shading experiment/10CC_shading_230302025.xlsx
+++ b/STORE_model/ML_model/data/shading experiment/10CC_shading_230302025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\ML_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\STORE_model\ML_model\data\shading experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD559F4A-A078-41CD-93F9-5F2AF8A8146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DBB186-9DCB-4472-9A5E-C0882B5FDD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="het growth" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="HET concentrations" sheetId="3" r:id="rId5"/>
     <sheet name="experiment plan" sheetId="5" r:id="rId6"/>
     <sheet name="starter FCM" sheetId="4" r:id="rId7"/>
+    <sheet name="Final FCM" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="227">
   <si>
     <t>1A3</t>
   </si>
@@ -618,6 +619,228 @@
   <si>
     <t>Heterotrophs cell ml-1</t>
   </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>All | Count</t>
+  </si>
+  <si>
+    <t>MED4</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>02-Well-A1.fcs</t>
+  </si>
+  <si>
+    <t>dil 1:500</t>
+  </si>
+  <si>
+    <t>dil 1:100</t>
+  </si>
+  <si>
+    <t>02-Well-A2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A7.fcs</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>02-Well-A11.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-A12.fcs</t>
+  </si>
+  <si>
+    <t>10^7</t>
+  </si>
+  <si>
+    <t>02-Well-B1.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-B7.fcs</t>
+  </si>
+  <si>
+    <t>10^8</t>
+  </si>
+  <si>
+    <t>02-Well-C1.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-C7.fcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED4 </t>
+  </si>
+  <si>
+    <t>02-Well-C8.fcs</t>
+  </si>
+  <si>
+    <t>sybr</t>
+  </si>
+  <si>
+    <t>02-Well-D1.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-D7.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E1.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-E7.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F1.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F2.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F3.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F4.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F5.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-F7.fcs</t>
+  </si>
+  <si>
+    <t>Alt</t>
+  </si>
+  <si>
+    <t>02-Well-G1.fcs</t>
+  </si>
+  <si>
+    <t>pseudo Alt</t>
+  </si>
+  <si>
+    <t>02-Well-G2.fcs</t>
+  </si>
+  <si>
+    <t>ntz</t>
+  </si>
+  <si>
+    <t>02-Well-G3.fcs</t>
+  </si>
+  <si>
+    <t>marino F3</t>
+  </si>
+  <si>
+    <t>02-Well-G4.fcs</t>
+  </si>
+  <si>
+    <t>roseo</t>
+  </si>
+  <si>
+    <t>02-Well-G5.fcs</t>
+  </si>
+  <si>
+    <t>phaeob</t>
+  </si>
+  <si>
+    <t>02-Well-G6.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-G7.fcs</t>
+  </si>
+  <si>
+    <t>02-Well-G8.fcs</t>
+  </si>
 </sst>
 </file>
 
@@ -627,9 +850,9 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,6 +958,18 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -924,7 +1159,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -973,7 +1208,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1013,10 +1248,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1055,6 +1286,21 @@
     </xf>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2874,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB40150-EDAC-41C4-8E47-67401EC79409}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="R8" sqref="M4:R8"/>
     </sheetView>
   </sheetViews>
@@ -2963,22 +3209,22 @@
       <c r="G4" s="23">
         <v>0.53086199999999995</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="P4" s="48" t="s">
+      <c r="P4" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="R4" s="45" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3004,22 +3250,22 @@
       <c r="G5" s="23">
         <v>0.53102300000000002</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="50">
+      <c r="N5" s="48">
         <v>40</v>
       </c>
-      <c r="O5" s="51">
+      <c r="O5" s="49">
         <v>1</v>
       </c>
-      <c r="P5" s="50">
+      <c r="P5" s="48">
         <v>0</v>
       </c>
-      <c r="Q5" s="50" t="s">
+      <c r="Q5" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="50"/>
+      <c r="R5" s="48"/>
     </row>
     <row r="6" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
@@ -3043,62 +3289,62 @@
       <c r="G6" s="23">
         <v>0.68685600000000002</v>
       </c>
-      <c r="M6" s="49" t="s">
+      <c r="M6" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="N6" s="50">
+      <c r="N6" s="48">
         <v>35</v>
       </c>
-      <c r="O6" s="52">
+      <c r="O6" s="50">
         <v>0.998</v>
       </c>
-      <c r="P6" s="50" t="s">
+      <c r="P6" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="Q6" s="50" t="s">
+      <c r="Q6" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="48" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="N7" s="50">
+      <c r="N7" s="48">
         <v>35</v>
       </c>
-      <c r="O7" s="52">
+      <c r="O7" s="50">
         <v>0.98299999999999998</v>
       </c>
-      <c r="P7" s="50" t="s">
+      <c r="P7" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="Q7" s="50" t="s">
+      <c r="Q7" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="R7" s="50" t="s">
+      <c r="R7" s="48" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="N8" s="50">
+      <c r="N8" s="48">
         <v>35</v>
       </c>
-      <c r="O8" s="52">
+      <c r="O8" s="50">
         <v>0.82499999999999996</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="P8" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="Q8" s="50" t="s">
+      <c r="Q8" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="R8" s="50" t="s">
+      <c r="R8" s="48" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3111,8 +3357,8 @@
       <c r="D10" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3120,8 +3366,8 @@
       <c r="B11" s="30"/>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:18" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3134,13 +3380,13 @@
       <c r="C12" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="38" t="s">
         <v>132</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="38" t="s">
         <v>135</v>
       </c>
       <c r="G12" s="33"/>
@@ -3168,18 +3414,18 @@
       <c r="B13" s="36">
         <v>40</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="43">
         <v>1</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="41" t="s">
         <v>136</v>
       </c>
       <c r="E13" s="37"/>
-      <c r="F13" s="41">
+      <c r="F13" s="39">
         <v>0</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="44"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="42"/>
       <c r="M13" s="14" t="s">
         <v>111</v>
       </c>
@@ -3203,20 +3449,20 @@
       <c r="B14" s="36">
         <v>35</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="44">
         <v>0.998</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="41" t="s">
         <v>139</v>
       </c>
       <c r="E14" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="42"/>
       <c r="M14" s="14" t="s">
         <v>112</v>
       </c>
@@ -3240,20 +3486,20 @@
       <c r="B15" s="36">
         <v>35</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="44">
         <v>0.98299999999999998</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="41" t="s">
         <v>142</v>
       </c>
       <c r="E15" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="44"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="42"/>
       <c r="M15" s="14" t="s">
         <v>113</v>
       </c>
@@ -3277,20 +3523,20 @@
       <c r="B16" s="36">
         <v>35</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="44">
         <v>0.82499999999999996</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="41" t="s">
         <v>145</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="44"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="42"/>
       <c r="M16" s="14" t="s">
         <v>114</v>
       </c>
@@ -4589,4 +4835,1491 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F1A38A-FE9B-4DAD-BE09-DA9FA1D11671}">
+  <dimension ref="A1:O54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="57" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="11" bestFit="1" customWidth="1"/>
+    <col min="517" max="517" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="11" bestFit="1" customWidth="1"/>
+    <col min="773" max="773" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="778" max="778" width="11" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1029" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1034" width="11" bestFit="1" customWidth="1"/>
+    <col min="1285" max="1285" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1290" width="11" bestFit="1" customWidth="1"/>
+    <col min="1541" max="1541" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1546" width="11" bestFit="1" customWidth="1"/>
+    <col min="1797" max="1797" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1802" max="1802" width="11" bestFit="1" customWidth="1"/>
+    <col min="2053" max="2053" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2058" width="11" bestFit="1" customWidth="1"/>
+    <col min="2309" max="2309" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2314" width="11" bestFit="1" customWidth="1"/>
+    <col min="2565" max="2565" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2570" width="11" bestFit="1" customWidth="1"/>
+    <col min="2821" max="2821" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2826" max="2826" width="11" bestFit="1" customWidth="1"/>
+    <col min="3077" max="3077" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3082" width="11" bestFit="1" customWidth="1"/>
+    <col min="3333" max="3333" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3338" width="11" bestFit="1" customWidth="1"/>
+    <col min="3589" max="3589" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3594" width="11" bestFit="1" customWidth="1"/>
+    <col min="3845" max="3845" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3850" width="11" bestFit="1" customWidth="1"/>
+    <col min="4101" max="4101" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4106" width="11" bestFit="1" customWidth="1"/>
+    <col min="4357" max="4357" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4362" width="11" bestFit="1" customWidth="1"/>
+    <col min="4613" max="4613" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4618" width="11" bestFit="1" customWidth="1"/>
+    <col min="4869" max="4869" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4874" max="4874" width="11" bestFit="1" customWidth="1"/>
+    <col min="5125" max="5125" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5130" width="11" bestFit="1" customWidth="1"/>
+    <col min="5381" max="5381" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5386" width="11" bestFit="1" customWidth="1"/>
+    <col min="5637" max="5637" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5642" width="11" bestFit="1" customWidth="1"/>
+    <col min="5893" max="5893" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5898" max="5898" width="11" bestFit="1" customWidth="1"/>
+    <col min="6149" max="6149" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6154" width="11" bestFit="1" customWidth="1"/>
+    <col min="6405" max="6405" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6410" width="11" bestFit="1" customWidth="1"/>
+    <col min="6661" max="6661" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6666" width="11" bestFit="1" customWidth="1"/>
+    <col min="6917" max="6917" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6922" max="6922" width="11" bestFit="1" customWidth="1"/>
+    <col min="7173" max="7173" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7178" width="11" bestFit="1" customWidth="1"/>
+    <col min="7429" max="7429" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7434" width="11" bestFit="1" customWidth="1"/>
+    <col min="7685" max="7685" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7690" width="11" bestFit="1" customWidth="1"/>
+    <col min="7941" max="7941" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7946" max="7946" width="11" bestFit="1" customWidth="1"/>
+    <col min="8197" max="8197" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8202" width="11" bestFit="1" customWidth="1"/>
+    <col min="8453" max="8453" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8458" width="11" bestFit="1" customWidth="1"/>
+    <col min="8709" max="8709" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8714" width="11" bestFit="1" customWidth="1"/>
+    <col min="8965" max="8965" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8970" max="8970" width="11" bestFit="1" customWidth="1"/>
+    <col min="9221" max="9221" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9226" width="11" bestFit="1" customWidth="1"/>
+    <col min="9477" max="9477" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9482" width="11" bestFit="1" customWidth="1"/>
+    <col min="9733" max="9733" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9738" width="11" bestFit="1" customWidth="1"/>
+    <col min="9989" max="9989" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9994" max="9994" width="11" bestFit="1" customWidth="1"/>
+    <col min="10245" max="10245" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10250" width="11" bestFit="1" customWidth="1"/>
+    <col min="10501" max="10501" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10506" width="11" bestFit="1" customWidth="1"/>
+    <col min="10757" max="10757" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10762" max="10762" width="11" bestFit="1" customWidth="1"/>
+    <col min="11013" max="11013" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11018" width="11" bestFit="1" customWidth="1"/>
+    <col min="11269" max="11269" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11274" width="11" bestFit="1" customWidth="1"/>
+    <col min="11525" max="11525" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11530" width="11" bestFit="1" customWidth="1"/>
+    <col min="11781" max="11781" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11786" max="11786" width="11" bestFit="1" customWidth="1"/>
+    <col min="12037" max="12037" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12042" width="11" bestFit="1" customWidth="1"/>
+    <col min="12293" max="12293" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12298" width="11" bestFit="1" customWidth="1"/>
+    <col min="12549" max="12549" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12554" width="11" bestFit="1" customWidth="1"/>
+    <col min="12805" max="12805" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12810" max="12810" width="11" bestFit="1" customWidth="1"/>
+    <col min="13061" max="13061" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13066" width="11" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13317" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13322" width="11" bestFit="1" customWidth="1"/>
+    <col min="13573" max="13573" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13578" width="11" bestFit="1" customWidth="1"/>
+    <col min="13829" max="13829" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13834" max="13834" width="11" bestFit="1" customWidth="1"/>
+    <col min="14085" max="14085" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14090" width="11" bestFit="1" customWidth="1"/>
+    <col min="14341" max="14341" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14346" width="11" bestFit="1" customWidth="1"/>
+    <col min="14597" max="14597" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14602" width="11" bestFit="1" customWidth="1"/>
+    <col min="14853" max="14853" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14858" max="14858" width="11" bestFit="1" customWidth="1"/>
+    <col min="15109" max="15109" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15114" width="11" bestFit="1" customWidth="1"/>
+    <col min="15365" max="15365" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15370" width="11" bestFit="1" customWidth="1"/>
+    <col min="15621" max="15621" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15626" width="11" bestFit="1" customWidth="1"/>
+    <col min="15877" max="15877" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15882" max="15882" width="11" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16138" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2">
+        <v>13022</v>
+      </c>
+      <c r="J2" s="56">
+        <f>F2*100/0.005</f>
+        <v>260440000</v>
+      </c>
+      <c r="N2" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3">
+        <v>9344</v>
+      </c>
+      <c r="J3" s="56">
+        <f t="shared" ref="J3:J24" si="0">F3*100/0.005</f>
+        <v>186880000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4">
+        <v>26370</v>
+      </c>
+      <c r="J4" s="56">
+        <f t="shared" si="0"/>
+        <v>527400000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5">
+        <v>8996</v>
+      </c>
+      <c r="J5" s="56">
+        <f t="shared" si="0"/>
+        <v>179920000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6">
+        <v>14506</v>
+      </c>
+      <c r="J6" s="56">
+        <f t="shared" si="0"/>
+        <v>290120000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7">
+        <v>13661</v>
+      </c>
+      <c r="J7" s="56">
+        <f t="shared" si="0"/>
+        <v>273220000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8">
+        <v>13576</v>
+      </c>
+      <c r="J8" s="56">
+        <f t="shared" si="0"/>
+        <v>271520000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="J9" s="56"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="56"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11">
+        <v>13531</v>
+      </c>
+      <c r="J11" s="56">
+        <f t="shared" si="0"/>
+        <v>270620000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12">
+        <v>11856</v>
+      </c>
+      <c r="J12" s="56">
+        <f t="shared" si="0"/>
+        <v>237120000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13">
+        <v>23</v>
+      </c>
+      <c r="J13" s="56">
+        <f t="shared" si="0"/>
+        <v>460000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14">
+        <v>12317</v>
+      </c>
+      <c r="J14" s="56">
+        <f t="shared" si="0"/>
+        <v>246340000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15">
+        <v>17076</v>
+      </c>
+      <c r="J15" s="56">
+        <f t="shared" si="0"/>
+        <v>341520000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16">
+        <v>18259</v>
+      </c>
+      <c r="J16" s="56">
+        <f t="shared" si="0"/>
+        <v>365180000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17">
+        <v>14521</v>
+      </c>
+      <c r="J17" s="56">
+        <f t="shared" si="0"/>
+        <v>290420000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18">
+        <v>10934</v>
+      </c>
+      <c r="J18" s="56">
+        <f t="shared" si="0"/>
+        <v>218680000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19">
+        <v>7509</v>
+      </c>
+      <c r="J19" s="56">
+        <f t="shared" si="0"/>
+        <v>150180000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20">
+        <v>11576</v>
+      </c>
+      <c r="J20" s="56">
+        <f t="shared" si="0"/>
+        <v>231520000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21">
+        <v>10867</v>
+      </c>
+      <c r="J21" s="56">
+        <f t="shared" si="0"/>
+        <v>217340000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22">
+        <v>10010</v>
+      </c>
+      <c r="J22" s="56">
+        <f t="shared" si="0"/>
+        <v>200200000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" t="s">
+        <v>187</v>
+      </c>
+      <c r="F23">
+        <v>12344</v>
+      </c>
+      <c r="J23" s="56">
+        <f t="shared" si="0"/>
+        <v>246880000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24">
+        <v>11811</v>
+      </c>
+      <c r="J24" s="56">
+        <f t="shared" si="0"/>
+        <v>236220000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F25">
+        <v>73438</v>
+      </c>
+      <c r="J25" s="56">
+        <f>F25*500/0.005</f>
+        <v>7343800000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="G26">
+        <v>14905</v>
+      </c>
+      <c r="J26" s="56"/>
+      <c r="K26" s="7">
+        <f>G26*100/0.005</f>
+        <v>298100000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27">
+        <v>9005</v>
+      </c>
+      <c r="J27" s="56"/>
+      <c r="K27" s="7">
+        <f t="shared" ref="K27:K46" si="1">G27*100/0.005</f>
+        <v>180100000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" t="s">
+        <v>194</v>
+      </c>
+      <c r="G28">
+        <v>12978</v>
+      </c>
+      <c r="J28" s="56"/>
+      <c r="K28" s="7">
+        <f t="shared" si="1"/>
+        <v>259560000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29">
+        <v>8859</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="K29" s="7">
+        <f t="shared" si="1"/>
+        <v>177180000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30">
+        <v>16088</v>
+      </c>
+      <c r="J30" s="56"/>
+      <c r="K30" s="7">
+        <f t="shared" si="1"/>
+        <v>321760000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31">
+        <v>11089</v>
+      </c>
+      <c r="J31" s="56"/>
+      <c r="K31" s="7">
+        <f t="shared" si="1"/>
+        <v>221780000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
+      <c r="G32">
+        <v>14079</v>
+      </c>
+      <c r="J32" s="56"/>
+      <c r="K32" s="7">
+        <f t="shared" si="1"/>
+        <v>281580000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" t="s">
+        <v>199</v>
+      </c>
+      <c r="G33">
+        <v>17960</v>
+      </c>
+      <c r="J33" s="56"/>
+      <c r="K33" s="7">
+        <f t="shared" si="1"/>
+        <v>359200000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34">
+        <v>14566</v>
+      </c>
+      <c r="J34" s="56"/>
+      <c r="K34" s="7">
+        <f t="shared" si="1"/>
+        <v>291320000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" t="s">
+        <v>201</v>
+      </c>
+      <c r="G35">
+        <v>15590</v>
+      </c>
+      <c r="J35" s="56"/>
+      <c r="K35" s="7">
+        <f t="shared" si="1"/>
+        <v>311800000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36">
+        <v>13893</v>
+      </c>
+      <c r="J36" s="56"/>
+      <c r="K36" s="7">
+        <f t="shared" si="1"/>
+        <v>277860000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37">
+        <v>17701</v>
+      </c>
+      <c r="J37" s="56"/>
+      <c r="K37" s="7">
+        <f t="shared" si="1"/>
+        <v>354020000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>204</v>
+      </c>
+      <c r="G38">
+        <v>17158</v>
+      </c>
+      <c r="J38" s="56"/>
+      <c r="K38" s="7">
+        <f t="shared" si="1"/>
+        <v>343160000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" t="s">
+        <v>205</v>
+      </c>
+      <c r="G39">
+        <v>17589</v>
+      </c>
+      <c r="J39" s="56"/>
+      <c r="K39" s="7">
+        <f t="shared" si="1"/>
+        <v>351780000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40">
+        <v>29502</v>
+      </c>
+      <c r="J40" s="56"/>
+      <c r="K40" s="7">
+        <f t="shared" si="1"/>
+        <v>590040000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" t="s">
+        <v>191</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>181</v>
+      </c>
+      <c r="E41" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41">
+        <v>34123</v>
+      </c>
+      <c r="J41" s="56"/>
+      <c r="K41" s="7">
+        <f t="shared" si="1"/>
+        <v>682460000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="G42">
+        <v>12951</v>
+      </c>
+      <c r="J42" s="56"/>
+      <c r="K42" s="7">
+        <f t="shared" si="1"/>
+        <v>259020000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" t="s">
+        <v>209</v>
+      </c>
+      <c r="G43">
+        <v>13243</v>
+      </c>
+      <c r="J43" s="56"/>
+      <c r="K43" s="7">
+        <f t="shared" si="1"/>
+        <v>264860000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" t="s">
+        <v>210</v>
+      </c>
+      <c r="G44">
+        <v>12238</v>
+      </c>
+      <c r="J44" s="56"/>
+      <c r="K44" s="7">
+        <f t="shared" si="1"/>
+        <v>244760000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" t="s">
+        <v>191</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" t="s">
+        <v>211</v>
+      </c>
+      <c r="G45">
+        <v>20952</v>
+      </c>
+      <c r="J45" s="56"/>
+      <c r="K45" s="7">
+        <f t="shared" si="1"/>
+        <v>419040000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" t="s">
+        <v>212</v>
+      </c>
+      <c r="G46">
+        <v>42784</v>
+      </c>
+      <c r="J46" s="56"/>
+      <c r="K46" s="7">
+        <f t="shared" si="1"/>
+        <v>855680000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" t="s">
+        <v>214</v>
+      </c>
+      <c r="G47">
+        <v>22308</v>
+      </c>
+      <c r="K47" s="7">
+        <f>G47*500/0.005</f>
+        <v>2230800000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" t="s">
+        <v>215</v>
+      </c>
+      <c r="E48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G48">
+        <v>5099</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" ref="K48:K54" si="2">G48*500/0.005</f>
+        <v>509900000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" t="s">
+        <v>191</v>
+      </c>
+      <c r="D49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E49" t="s">
+        <v>218</v>
+      </c>
+      <c r="G49">
+        <v>21316</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="2"/>
+        <v>2131600000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" t="s">
+        <v>220</v>
+      </c>
+      <c r="G50">
+        <v>30745</v>
+      </c>
+      <c r="K50" s="7">
+        <f t="shared" si="2"/>
+        <v>3074500000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" t="s">
+        <v>191</v>
+      </c>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
+      <c r="E51" t="s">
+        <v>222</v>
+      </c>
+      <c r="G51">
+        <v>54750</v>
+      </c>
+      <c r="K51" s="7">
+        <f t="shared" si="2"/>
+        <v>5475000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" t="s">
+        <v>224</v>
+      </c>
+      <c r="G52">
+        <v>4204</v>
+      </c>
+      <c r="K52" s="7">
+        <f t="shared" si="2"/>
+        <v>420400000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>225</v>
+      </c>
+      <c r="G53">
+        <v>36748</v>
+      </c>
+      <c r="K53" s="7">
+        <f t="shared" si="2"/>
+        <v>3674800000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" t="s">
+        <v>191</v>
+      </c>
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" t="s">
+        <v>226</v>
+      </c>
+      <c r="G54">
+        <v>72533</v>
+      </c>
+      <c r="K54" s="7">
+        <f t="shared" si="2"/>
+        <v>7253300000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>